<commit_message>
Updated time plan and budget
</commit_message>
<xml_diff>
--- a/Tidsplan/Budget beregninger.xlsx
+++ b/Tidsplan/Budget beregninger.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="0" windowWidth="19200" windowHeight="23560" tabRatio="500"/>
+    <workbookView xWindow="-75" yWindow="0" windowWidth="19200" windowHeight="18240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Software developer (internal price)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Fase</t>
   </si>
@@ -57,22 +54,52 @@
     <t>pr dag</t>
   </si>
   <si>
-    <t>Fase 8</t>
-  </si>
-  <si>
-    <t>Fase 1-2</t>
-  </si>
-  <si>
-    <t>Fase 4-7</t>
-  </si>
-  <si>
-    <t>Fase 9</t>
-  </si>
-  <si>
     <t>Fase 10</t>
   </si>
   <si>
-    <t>Total:</t>
+    <t>Arbejdsdage på en uge</t>
+  </si>
+  <si>
+    <t>To mand i service center</t>
+  </si>
+  <si>
+    <t>It-support</t>
+  </si>
+  <si>
+    <t>Software udvikler (intern pris)</t>
+  </si>
+  <si>
+    <t>Noter</t>
+  </si>
+  <si>
+    <t>Vagttillæg</t>
+  </si>
+  <si>
+    <t>Fase 8-9</t>
+  </si>
+  <si>
+    <t>Total (u. prod.)</t>
+  </si>
+  <si>
+    <t>Total (m. prod)</t>
+  </si>
+  <si>
+    <t>Fase 7</t>
+  </si>
+  <si>
+    <t>Fase 1-4</t>
+  </si>
+  <si>
+    <t>Fase 5-6</t>
+  </si>
+  <si>
+    <t>Garantiservice pr. år</t>
+  </si>
+  <si>
+    <t>Hver person får 1000kr i vagttillæg pr. dag (24x7)</t>
+  </si>
+  <si>
+    <t>Produktionspris</t>
   </si>
 </sst>
 </file>
@@ -143,9 +170,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
@@ -156,18 +184,23 @@
     <cellStyle name="Besøgt link" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -493,120 +526,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:K27"/>
+  <dimension ref="A3:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:11">
-      <c r="I5" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
         <v>4</v>
       </c>
-      <c r="J5">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4000</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3000</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="K5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="I6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>4000</v>
-      </c>
-      <c r="K6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="I7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7">
-        <v>8</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
-        <v>8.6</v>
+        <v>17.2</v>
       </c>
       <c r="C9">
-        <f>B9*J$5</f>
-        <v>43</v>
+        <f>B9*I$4</f>
+        <v>86</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E9" s="1">
-        <f>J$6</f>
+        <f>I$6</f>
         <v>4000</v>
       </c>
       <c r="F9" s="1">
         <f>E9*C9*D9</f>
-        <v>1204000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>3440000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10">
-        <v>39.4</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="C10">
-        <f>B10*J$5</f>
-        <v>197</v>
+        <f>B10*I$4</f>
+        <v>176</v>
       </c>
       <c r="D10">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1">
-        <f>J$6</f>
+        <f>I$6</f>
         <v>4000</v>
       </c>
       <c r="F10" s="1">
         <f>E10*C10*D10</f>
-        <v>15760000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>10560000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -614,114 +682,114 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C15" si="0">B11*J$5</f>
+        <f>B11*I$4</f>
         <v>65</v>
       </c>
       <c r="D11">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" ref="E11:E15" si="1">J$6</f>
+        <f t="shared" ref="E11:E15" si="0">I$6</f>
         <v>4000</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ref="F11:F15" si="2">E11*C11*D11</f>
-        <v>7800000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <f t="shared" ref="F11:F15" si="1">E11*C11*D11</f>
+        <v>5200000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="B12">
-        <v>13</v>
+        <v>6.4</v>
       </c>
       <c r="C12">
+        <f>B12*I$4</f>
+        <v>32</v>
+      </c>
+      <c r="D12">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="D12">
-        <v>70</v>
-      </c>
-      <c r="E12" s="1">
+        <v>4000</v>
+      </c>
+      <c r="F12" s="1">
         <f t="shared" si="1"/>
-        <v>4000</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="2"/>
-        <v>18200000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>5120000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13">
-        <v>8.8000000000000007</v>
+        <v>6.2</v>
       </c>
       <c r="C13">
+        <f>B13*I$4</f>
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="D13">
-        <v>30</v>
-      </c>
-      <c r="E13" s="1">
+        <v>4000</v>
+      </c>
+      <c r="F13" s="1">
         <f t="shared" si="1"/>
-        <v>4000</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="2"/>
-        <v>5280000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>2480000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
       <c r="B14">
-        <v>8.6</v>
+        <v>30</v>
       </c>
       <c r="C14">
+        <f>B14*I$4</f>
+        <v>150</v>
+      </c>
+      <c r="D14">
+        <v>40</v>
+      </c>
+      <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="D14">
-        <v>20</v>
-      </c>
-      <c r="E14" s="1">
+        <v>4000</v>
+      </c>
+      <c r="F14" s="1">
         <f t="shared" si="1"/>
-        <v>4000</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" si="2"/>
-        <v>3440000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>24000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8</v>
       </c>
       <c r="B15">
-        <v>8.8000000000000007</v>
+        <v>21.8</v>
       </c>
       <c r="C15">
+        <f>B15*I$4</f>
+        <v>109</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="D15">
-        <v>20</v>
-      </c>
-      <c r="E15" s="1">
+        <v>4000</v>
+      </c>
+      <c r="F15" s="1">
         <f t="shared" si="1"/>
-        <v>4000</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" si="2"/>
-        <v>3520000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>6540000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
@@ -729,14 +797,14 @@
         <v>521.79999999999995</v>
       </c>
       <c r="C16">
-        <f>B16*J$5</f>
+        <f>B16*I$4</f>
         <v>2609</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
       <c r="E16" s="1">
-        <f>J$6</f>
+        <f>I$6</f>
         <v>4000</v>
       </c>
       <c r="F16" s="1">
@@ -744,7 +812,7 @@
         <v>31308000</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
@@ -752,73 +820,174 @@
         <v>1043.5999999999999</v>
       </c>
       <c r="C17">
-        <f>B17*J$5</f>
-        <v>5218</v>
+        <f>B17*I$5</f>
+        <v>7305.1999999999989</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" s="1">
-        <f>J$6</f>
-        <v>4000</v>
+        <f>I$8</f>
+        <v>1000</v>
       </c>
       <c r="F17" s="1">
         <f>E17*C17*D17</f>
-        <v>41744000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="E20" t="s">
+        <v>14610399.999999998</v>
+      </c>
+      <c r="G17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>1043.5999999999999</v>
+      </c>
+      <c r="C18">
+        <f>B18*I$4</f>
+        <v>5218</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <f>I$7</f>
+        <v>3000</v>
+      </c>
+      <c r="F18" s="1">
+        <f>E18*C18*D18</f>
+        <v>31308000</v>
+      </c>
+      <c r="G18" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="1">
-        <f>SUM(F9:F10)</f>
-        <v>16964000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="E21" t="s">
-        <v>14</v>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>52</v>
+      </c>
+      <c r="C21">
+        <f>B21*I$4</f>
+        <v>260</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1">
+        <f>I8</f>
+        <v>1000</v>
       </c>
       <c r="F21" s="1">
-        <f>SUM(F11:F14)</f>
-        <v>34720000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="E22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="1">
-        <f>F15</f>
-        <v>3520000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="E23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="1">
-        <f>F16</f>
-        <v>31308000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <f>E21*C21*D21</f>
+        <v>520000</v>
+      </c>
+      <c r="G21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F24" s="1">
-        <f>F17</f>
-        <v>41744000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="E27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="1">
-        <f>SUM(F9:F17)</f>
-        <v>128256000</v>
+        <f>SUM(F9:F11)</f>
+        <v>19200000</v>
+      </c>
+      <c r="G24" s="2">
+        <f>F24/F$31</f>
+        <v>0.37795275590551181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="1">
+        <f>SUM(F12:F13)</f>
+        <v>7600000</v>
+      </c>
+      <c r="G25" s="2">
+        <f>F25/F$31</f>
+        <v>0.14960629921259844</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="1">
+        <f>F14</f>
+        <v>24000000</v>
+      </c>
+      <c r="G26" s="2">
+        <f>F26/F$31</f>
+        <v>0.47244094488188976</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="1">
+        <f>F15+F16</f>
+        <v>37848000</v>
+      </c>
+      <c r="G28" s="2">
+        <f>F28/F$32</f>
+        <v>0.28125891753067628</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="1">
+        <f>F17+F18</f>
+        <v>45918400</v>
+      </c>
+      <c r="G29" s="2">
+        <f>F29/F$32</f>
+        <v>0.34123228383905641</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="1">
+        <f>SUM(F24:F26)</f>
+        <v>50800000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="1">
+        <f>SUM(F9:F18)</f>
+        <v>134566400</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="1">
+        <f>F32-F31</f>
+        <v>83766400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tilføjet budget til SEMP
</commit_message>
<xml_diff>
--- a/Tidsplan/Budget beregninger.xlsx
+++ b/Tidsplan/Budget beregninger.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GIT\TISYE\Tidsplan\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="0" windowWidth="19200" windowHeight="18240" tabRatio="500"/>
+    <workbookView xWindow="-72" yWindow="0" windowWidth="19200" windowHeight="18240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -176,22 +181,22 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besøgt link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -199,6 +204,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -528,20 +536,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" t="s">
         <v>8</v>
       </c>
@@ -552,7 +560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H4" t="s">
         <v>12</v>
       </c>
@@ -563,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H5" t="s">
         <v>3</v>
       </c>
@@ -574,7 +582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H6" t="s">
         <v>15</v>
       </c>
@@ -585,7 +593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H7" t="s">
         <v>14</v>
       </c>
@@ -596,7 +604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -628,7 +636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -636,7 +644,7 @@
         <v>17.2</v>
       </c>
       <c r="C9">
-        <f>B9*I$4</f>
+        <f t="shared" ref="C9:C16" si="0">B9*I$4</f>
         <v>86</v>
       </c>
       <c r="D9">
@@ -651,7 +659,7 @@
         <v>3440000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -659,7 +667,7 @@
         <v>35.200000000000003</v>
       </c>
       <c r="C10">
-        <f>B10*I$4</f>
+        <f t="shared" si="0"/>
         <v>176</v>
       </c>
       <c r="D10">
@@ -674,7 +682,7 @@
         <v>10560000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -682,22 +690,22 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <f>B11*I$4</f>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="D11">
         <v>20</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" ref="E11:E15" si="0">I$6</f>
+        <f t="shared" ref="E11:E15" si="1">I$6</f>
         <v>4000</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ref="F11:F15" si="1">E11*C11*D11</f>
+        <f t="shared" ref="F11:F15" si="2">E11*C11*D11</f>
         <v>5200000</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
@@ -705,22 +713,22 @@
         <v>6.4</v>
       </c>
       <c r="C12">
-        <f>B12*I$4</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="D12">
         <v>40</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4000</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5120000</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -728,22 +736,22 @@
         <v>6.2</v>
       </c>
       <c r="C13">
-        <f>B13*I$4</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="D13">
         <v>20</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4000</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2480000</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -751,22 +759,22 @@
         <v>30</v>
       </c>
       <c r="C14">
-        <f>B14*I$4</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="D14">
         <v>40</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4000</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24000000</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -774,22 +782,22 @@
         <v>21.8</v>
       </c>
       <c r="C15">
-        <f>B15*I$4</f>
+        <f t="shared" si="0"/>
         <v>109</v>
       </c>
       <c r="D15">
         <v>15</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4000</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6540000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
@@ -797,7 +805,7 @@
         <v>521.79999999999995</v>
       </c>
       <c r="C16">
-        <f>B16*I$4</f>
+        <f t="shared" si="0"/>
         <v>2609</v>
       </c>
       <c r="D16">
@@ -812,7 +820,7 @@
         <v>31308000</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
@@ -838,7 +846,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10</v>
       </c>
@@ -864,15 +872,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10</v>
       </c>
@@ -898,7 +906,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>22</v>
       </c>
@@ -911,7 +919,7 @@
         <v>0.37795275590551181</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>23</v>
       </c>
@@ -924,7 +932,7 @@
         <v>0.14960629921259844</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
         <v>21</v>
       </c>
@@ -937,7 +945,7 @@
         <v>0.47244094488188976</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>18</v>
       </c>
@@ -950,7 +958,7 @@
         <v>0.28125891753067628</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>11</v>
       </c>
@@ -963,7 +971,7 @@
         <v>0.34123228383905641</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E31" t="s">
         <v>19</v>
       </c>
@@ -972,7 +980,7 @@
         <v>50800000</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E32" t="s">
         <v>20</v>
       </c>
@@ -981,7 +989,7 @@
         <v>134566400</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E33" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Læst, og småting rettet til
Stavefejl, mærkelige formuleringer rettet.
En tabel er oprettet til refrenced documents.
</commit_message>
<xml_diff>
--- a/Tidsplan/Budget beregninger.xlsx
+++ b/Tidsplan/Budget beregninger.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GIT\TISYE\Tidsplan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasorensen\Desktop\IHA-student\1. Civil\TISYE\Tidsplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-72" yWindow="0" windowWidth="19200" windowHeight="18240" tabRatio="500"/>
+    <workbookView xWindow="-75" yWindow="0" windowWidth="19200" windowHeight="18240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -181,22 +181,22 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -536,20 +536,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
         <v>8</v>
       </c>
@@ -560,7 +560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
         <v>12</v>
       </c>
@@ -571,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
         <v>3</v>
       </c>
@@ -582,7 +582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
         <v>15</v>
       </c>
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
         <v>14</v>
       </c>
@@ -604,7 +604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -636,7 +636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -659,7 +659,7 @@
         <v>3440000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -682,7 +682,7 @@
         <v>10560000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -705,7 +705,7 @@
         <v>5200000</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -728,7 +728,7 @@
         <v>5120000</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -751,7 +751,7 @@
         <v>2480000</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -774,7 +774,7 @@
         <v>24000000</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8</v>
       </c>
@@ -797,7 +797,7 @@
         <v>6540000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
@@ -820,7 +820,7 @@
         <v>31308000</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
@@ -846,7 +846,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
@@ -872,15 +872,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10</v>
       </c>
@@ -906,7 +906,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>22</v>
       </c>
@@ -918,8 +918,12 @@
         <f>F24/F$31</f>
         <v>0.37795275590551181</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" s="2">
+        <f>F24/F$32</f>
+        <v>0.14268049082088843</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>23</v>
       </c>
@@ -931,8 +935,12 @@
         <f>F25/F$31</f>
         <v>0.14960629921259844</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" s="2">
+        <f t="shared" ref="H25:H29" si="3">F25/F$32</f>
+        <v>5.6477694283268334E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>21</v>
       </c>
@@ -944,8 +952,15 @@
         <f>F26/F$31</f>
         <v>0.47244094488188976</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" s="2">
+        <f t="shared" si="3"/>
+        <v>0.17835061352611054</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>18</v>
       </c>
@@ -953,12 +968,13 @@
         <f>F15+F16</f>
         <v>37848000</v>
       </c>
-      <c r="G28" s="2">
-        <f>F28/F$32</f>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2">
+        <f t="shared" si="3"/>
         <v>0.28125891753067628</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>11</v>
       </c>
@@ -966,12 +982,13 @@
         <f>F17+F18</f>
         <v>45918400</v>
       </c>
-      <c r="G29" s="2">
-        <f>F29/F$32</f>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2">
+        <f t="shared" si="3"/>
         <v>0.34123228383905641</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>19</v>
       </c>
@@ -980,7 +997,7 @@
         <v>50800000</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>20</v>
       </c>
@@ -989,7 +1006,7 @@
         <v>134566400</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>26</v>
       </c>

</xml_diff>